<commit_message>
changing days to week format for timeseries data
</commit_message>
<xml_diff>
--- a/PennStateCovidTables.xlsx
+++ b/PennStateCovidTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samon\Documents\group_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valerielindstrom/Desktop/group_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91237F1B-7675-45D7-8F74-6F3EE46A95C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806025CC-C9A3-C244-BC1B-B4A4B823562A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{925EDFE9-5936-4DE2-955A-4EE15794EB9C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{925EDFE9-5936-4DE2-955A-4EE15794EB9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Total_Positive</t>
   </si>
   <si>
-    <t>Week_Start</t>
-  </si>
-  <si>
-    <t>Week_End</t>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>8/7/2020 - 8/13/2020</t>
+  </si>
+  <si>
+    <t>8/14/2020 - 8/20/2020</t>
+  </si>
+  <si>
+    <t>8/21/2020 - 8/27/2020</t>
+  </si>
+  <si>
+    <t>8/28/2020 - 9/3/2020</t>
+  </si>
+  <si>
+    <t>9/4/2020 - 9/10/2020</t>
+  </si>
+  <si>
+    <t>9/25/2020 - 10/1/2020</t>
+  </si>
+  <si>
+    <t>10/2/2020 - 10/8/2020</t>
+  </si>
+  <si>
+    <t>10/9/2020 - 10/15/2020</t>
+  </si>
+  <si>
+    <t>10/16/2020 - 10/22/2020</t>
+  </si>
+  <si>
+    <t>10/23/2020 - 10/29/2020</t>
+  </si>
+  <si>
+    <t>10/30/2020 - 11/5/2020</t>
+  </si>
+  <si>
+    <t>11/6/2020 - 11/12/2020</t>
+  </si>
+  <si>
+    <t>11/20/2020 - 11/22/2020</t>
+  </si>
+  <si>
+    <t>11/13/2020 - 11/19/2020</t>
+  </si>
+  <si>
+    <t>9/18/2020 - 9/24/2020</t>
+  </si>
+  <si>
+    <t>9/11/2020 - 9/17/2020</t>
   </si>
 </sst>
 </file>
@@ -78,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,208 +441,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCC79FD-F36C-46CC-8B18-BD1BA763856A}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44050</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44056</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44057</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44063</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44064</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44070</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44071</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44077</v>
-      </c>
-      <c r="C5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44078</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44084</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>575</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44085</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44091</v>
-      </c>
-      <c r="C7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>44092</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
         <v>666</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>44099</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44105</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>466</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>44106</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44112</v>
-      </c>
-      <c r="C10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>44113</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44119</v>
-      </c>
-      <c r="C11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>44120</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44126</v>
-      </c>
-      <c r="C12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>44127</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44133</v>
-      </c>
-      <c r="C13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>44134</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44140</v>
-      </c>
-      <c r="C14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>44141</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44147</v>
-      </c>
-      <c r="C15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>44148</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44154</v>
-      </c>
-      <c r="C16">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>379</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>44155</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44157</v>
-      </c>
-      <c r="C17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>